<commit_message>
problem 9 success rate
</commit_message>
<xml_diff>
--- a/output/junior/9_count.xlsx
+++ b/output/junior/9_count.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>list</t>
   </si>
@@ -22,19 +22,25 @@
     <t>count</t>
   </si>
   <si>
+    <t>success</t>
+  </si>
+  <si>
     <t>['00_02', '00_05']</t>
   </si>
   <si>
-    <t>['00_02', '05_00']</t>
+    <t>['00_02', '00_09']</t>
+  </si>
+  <si>
+    <t>['00_02', '05_06']</t>
   </si>
   <si>
     <t>['00_02']</t>
   </si>
   <si>
-    <t>['00_05', '02_00']</t>
-  </si>
-  <si>
-    <t>['00_05', '03_02']</t>
+    <t>['00_05', '02_03']</t>
+  </si>
+  <si>
+    <t>['00_05', '02_08']</t>
   </si>
   <si>
     <t>['00_05', '06_07']</t>
@@ -43,13 +49,28 @@
     <t>['00_09']</t>
   </si>
   <si>
-    <t>['01_03', '06_05']</t>
-  </si>
-  <si>
-    <t>['01_03', '07_04']</t>
-  </si>
-  <si>
-    <t>['01_04', '05_03']</t>
+    <t>['01_03', '01_08']</t>
+  </si>
+  <si>
+    <t>['01_03', '03_06']</t>
+  </si>
+  <si>
+    <t>['01_03', '04_07']</t>
+  </si>
+  <si>
+    <t>['01_03', '05_06']</t>
+  </si>
+  <si>
+    <t>['01_03', '07_09']</t>
+  </si>
+  <si>
+    <t>['01_04', '03_05']</t>
+  </si>
+  <si>
+    <t>['01_04', '05_07']</t>
+  </si>
+  <si>
+    <t>['01_05', '01_08']</t>
   </si>
   <si>
     <t>['01_05', '02_06']</t>
@@ -58,55 +79,49 @@
     <t>['01_05', '02_09']</t>
   </si>
   <si>
-    <t>['01_06', '08_03']</t>
-  </si>
-  <si>
-    <t>['01_07', '07_04']</t>
+    <t>['01_06', '02_08']</t>
+  </si>
+  <si>
+    <t>['01_06', '03_08']</t>
+  </si>
+  <si>
+    <t>['01_07', '04_07']</t>
   </si>
   <si>
     <t>['01_08', '02_08']</t>
   </si>
   <si>
-    <t>['01_08', '03_01']</t>
+    <t>['01_08', '04_06']</t>
   </si>
   <si>
     <t>['01_08']</t>
   </si>
   <si>
-    <t>['02_00', '06_05']</t>
-  </si>
-  <si>
-    <t>['02_00', '09_00']</t>
-  </si>
-  <si>
-    <t>['02_05', '06_03']</t>
+    <t>['02_03', '05_07']</t>
+  </si>
+  <si>
+    <t>['02_05', '03_06']</t>
   </si>
   <si>
     <t>['02_05', '06_09']</t>
   </si>
   <si>
-    <t>['02_05', '09_06']</t>
-  </si>
-  <si>
     <t>['02_06', '05_09']</t>
   </si>
   <si>
-    <t>['02_06', '09_05']</t>
-  </si>
-  <si>
-    <t>['02_07', '07_04']</t>
-  </si>
-  <si>
-    <t>['02_07', '07_05']</t>
-  </si>
-  <si>
-    <t>['02_08', '00_05']</t>
+    <t>['02_07', '04_07']</t>
+  </si>
+  <si>
+    <t>['02_07', '05_07']</t>
   </si>
   <si>
     <t>['02_08', '03_05']</t>
   </si>
   <si>
-    <t>['02_08', '09_07']</t>
+    <t>['02_08', '04_06']</t>
+  </si>
+  <si>
+    <t>['02_08', '07_09']</t>
   </si>
   <si>
     <t>['02_08']</t>
@@ -115,22 +130,16 @@
     <t>['02_09', '05_06']</t>
   </si>
   <si>
-    <t>['02_09', '06_05']</t>
-  </si>
-  <si>
-    <t>['02_09', '09_05']</t>
-  </si>
-  <si>
-    <t>['03_01', '03_06']</t>
+    <t>['02_09', '05_09']</t>
+  </si>
+  <si>
+    <t>['02_09', '06_07']</t>
   </si>
   <si>
     <t>['03_01']</t>
   </si>
   <si>
-    <t>['04_06', '02_08']</t>
-  </si>
-  <si>
-    <t>['04_06', '07_06']</t>
+    <t>['04_06', '06_07']</t>
   </si>
   <si>
     <t>['04_06']</t>
@@ -142,103 +151,31 @@
     <t>['05_00']</t>
   </si>
   <si>
-    <t>['05_01', '01_08']</t>
-  </si>
-  <si>
-    <t>['05_02', '03_06']</t>
-  </si>
-  <si>
-    <t>['05_02', '06_09']</t>
-  </si>
-  <si>
-    <t>['05_02', '09_06']</t>
-  </si>
-  <si>
-    <t>['05_06', '02_09']</t>
-  </si>
-  <si>
-    <t>['05_06', '09_02']</t>
-  </si>
-  <si>
-    <t>['05_07', '04_01']</t>
-  </si>
-  <si>
-    <t>['05_09', '05_07']</t>
-  </si>
-  <si>
-    <t>['06_01', '02_08']</t>
+    <t>['05_06', '06_07']</t>
+  </si>
+  <si>
+    <t>['05_07', '05_09']</t>
+  </si>
+  <si>
+    <t>['05_09', '06_07']</t>
   </si>
   <si>
     <t>['06_01']</t>
   </si>
   <si>
-    <t>['06_02', '09_05']</t>
-  </si>
-  <si>
-    <t>['06_04', '08_01']</t>
-  </si>
-  <si>
-    <t>['06_05', '02_09']</t>
-  </si>
-  <si>
-    <t>['06_05', '09_02']</t>
-  </si>
-  <si>
     <t>['06_07']</t>
   </si>
   <si>
-    <t>['06_09', '02_05']</t>
-  </si>
-  <si>
-    <t>['07_05', '02_03']</t>
-  </si>
-  <si>
-    <t>['07_06', '04_06']</t>
-  </si>
-  <si>
-    <t>['07_06', '05_06']</t>
-  </si>
-  <si>
-    <t>['07_06', '06_05']</t>
-  </si>
-  <si>
-    <t>['07_09', '01_03']</t>
-  </si>
-  <si>
-    <t>['08_01', '06_04']</t>
-  </si>
-  <si>
     <t>['08_01']</t>
   </si>
   <si>
-    <t>['08_03', '01_06']</t>
-  </si>
-  <si>
     <t>['08_03']</t>
   </si>
   <si>
-    <t>['09_02', '05_06']</t>
-  </si>
-  <si>
-    <t>['09_02', '06_05']</t>
-  </si>
-  <si>
-    <t>['09_02', '07_06']</t>
-  </si>
-  <si>
-    <t>['09_05', '02_06']</t>
-  </si>
-  <si>
-    <t>['09_05', '06_02']</t>
-  </si>
-  <si>
-    <t>['09_05', '06_07']</t>
-  </si>
-  <si>
-    <t>['09_06', '02_05']</t>
-  </si>
-  <si>
-    <t>['09_06', '05_02']</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -596,829 +533,718 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C33">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C34">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>158</v>
+      </c>
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C46">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C47">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C48">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="1">
-        <v>50</v>
-      </c>
-      <c r="B52" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="1">
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="1">
-        <v>52</v>
-      </c>
-      <c r="B54" t="s">
-        <v>53</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="1">
-        <v>53</v>
-      </c>
-      <c r="B55" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="1">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
-        <v>55</v>
-      </c>
-      <c r="C56">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="1">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="1">
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
-        <v>57</v>
-      </c>
-      <c r="C58">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="1">
-        <v>57</v>
-      </c>
-      <c r="B59" t="s">
-        <v>58</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="1">
-        <v>58</v>
-      </c>
-      <c r="B60" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="1">
-        <v>59</v>
-      </c>
-      <c r="B61" t="s">
-        <v>60</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="1">
-        <v>60</v>
-      </c>
-      <c r="B62" t="s">
-        <v>61</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="1">
-        <v>61</v>
-      </c>
-      <c r="B63" t="s">
-        <v>62</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="1">
-        <v>62</v>
-      </c>
-      <c r="B64" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1">
-        <v>63</v>
-      </c>
-      <c r="B65" t="s">
-        <v>64</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="1">
-        <v>64</v>
-      </c>
-      <c r="B66" t="s">
-        <v>65</v>
-      </c>
-      <c r="C66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1">
-        <v>65</v>
-      </c>
-      <c r="B67" t="s">
-        <v>66</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="1">
-        <v>66</v>
-      </c>
-      <c r="B68" t="s">
-        <v>67</v>
-      </c>
-      <c r="C68">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1">
-        <v>67</v>
-      </c>
-      <c r="B69" t="s">
-        <v>68</v>
-      </c>
-      <c r="C69">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1">
-        <v>68</v>
-      </c>
-      <c r="B70" t="s">
-        <v>69</v>
-      </c>
-      <c r="C70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1">
-        <v>69</v>
-      </c>
-      <c r="B71" t="s">
-        <v>70</v>
-      </c>
-      <c r="C71">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="1">
-        <v>70</v>
-      </c>
-      <c r="B72" t="s">
-        <v>71</v>
-      </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="1">
-        <v>71</v>
-      </c>
-      <c r="B73" t="s">
-        <v>72</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="1">
-        <v>72</v>
-      </c>
-      <c r="B74" t="s">
-        <v>73</v>
-      </c>
-      <c r="C74">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="1">
-        <v>73</v>
-      </c>
-      <c r="B75" t="s">
-        <v>74</v>
-      </c>
-      <c r="C75">
-        <v>6</v>
+      <c r="D51" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>